<commit_message>
update 1 Julky 23
</commit_message>
<xml_diff>
--- a/OMM-Task4.xlsx
+++ b/OMM-Task4.xlsx
@@ -16,25 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="9">
-  <si>
-    <t>CooA.wav</t>
-  </si>
-  <si>
-    <t>CooB_-20dB.wav</t>
-  </si>
-  <si>
-    <t>CooB_-15dB.wav</t>
-  </si>
-  <si>
-    <t>CooB_-10dB.wav</t>
-  </si>
-  <si>
-    <t>CooB_-5dB.wav</t>
-  </si>
-  <si>
-    <t>CooB.wav</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="9">
   <si>
     <t>Sound1</t>
   </si>
@@ -43,6 +25,24 @@
   </si>
   <si>
     <t>Position_Target</t>
+  </si>
+  <si>
+    <t>Avg16.wav</t>
+  </si>
+  <si>
+    <t>Coo_01.wav</t>
+  </si>
+  <si>
+    <t>Coo_01-20dB.wav</t>
+  </si>
+  <si>
+    <t>Coo_01-15dB.wav</t>
+  </si>
+  <si>
+    <t>Coo_01-10dB.wav</t>
+  </si>
+  <si>
+    <t>Coo_01-5dB.wav</t>
   </si>
 </sst>
 </file>
@@ -391,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C165"/>
+  <dimension ref="A1:C321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="C102" sqref="C102:C121"/>
+    <sheetView tabSelected="1" topLeftCell="A304" workbookViewId="0">
+      <selection activeCell="A258" sqref="A258:C321"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,21 +406,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -428,10 +428,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -439,10 +439,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C5">
         <v>2</v>
@@ -461,10 +461,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -472,10 +472,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C7">
         <v>2</v>
@@ -483,10 +483,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -494,10 +494,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C9">
         <v>2</v>
@@ -505,10 +505,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B10" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C10">
         <v>1</v>
@@ -516,10 +516,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C11">
         <v>2</v>
@@ -527,10 +527,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B12" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -538,10 +538,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C13">
         <v>2</v>
@@ -549,10 +549,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B14" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C14">
         <v>1</v>
@@ -560,10 +560,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C15">
         <v>2</v>
@@ -571,10 +571,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B16" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C16">
         <v>1</v>
@@ -582,10 +582,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C17">
         <v>2</v>
@@ -593,10 +593,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C18">
         <v>1</v>
@@ -604,10 +604,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C19">
         <v>2</v>
@@ -615,10 +615,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -626,10 +626,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C21">
         <v>2</v>
@@ -637,10 +637,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C22">
         <v>1</v>
@@ -648,10 +648,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C23">
         <v>2</v>
@@ -659,10 +659,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B24" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C24">
         <v>1</v>
@@ -670,10 +670,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C25">
         <v>2</v>
@@ -681,10 +681,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C26">
         <v>1</v>
@@ -692,10 +692,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C27">
         <v>2</v>
@@ -703,10 +703,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B28" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C28">
         <v>1</v>
@@ -714,10 +714,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C29">
         <v>2</v>
@@ -725,10 +725,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B30" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C30">
         <v>1</v>
@@ -736,10 +736,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -747,10 +747,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B32" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C32">
         <v>1</v>
@@ -758,10 +758,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C33">
         <v>2</v>
@@ -769,10 +769,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C34">
         <v>1</v>
@@ -780,10 +780,10 @@
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C35">
         <v>2</v>
@@ -791,10 +791,10 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B36" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C36">
         <v>1</v>
@@ -802,10 +802,10 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -813,10 +813,10 @@
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B38" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C38">
         <v>1</v>
@@ -824,10 +824,10 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C39">
         <v>2</v>
@@ -835,10 +835,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C40">
         <v>1</v>
@@ -846,10 +846,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C41">
         <v>2</v>
@@ -857,10 +857,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C42">
         <v>1</v>
@@ -868,10 +868,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C43">
         <v>2</v>
@@ -879,10 +879,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B44" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C44">
         <v>1</v>
@@ -890,10 +890,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C45">
         <v>2</v>
@@ -901,10 +901,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B46" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C46">
         <v>1</v>
@@ -912,10 +912,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C47">
         <v>2</v>
@@ -923,10 +923,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B48" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C48">
         <v>1</v>
@@ -934,10 +934,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -945,10 +945,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B50" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -956,10 +956,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C51">
         <v>2</v>
@@ -967,10 +967,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B52" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C52">
         <v>1</v>
@@ -978,10 +978,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C53">
         <v>2</v>
@@ -989,10 +989,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B54" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C54">
         <v>1</v>
@@ -1000,10 +1000,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C55">
         <v>2</v>
@@ -1011,10 +1011,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B56" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C56">
         <v>1</v>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C57">
         <v>2</v>
@@ -1033,10 +1033,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B58" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C58">
         <v>1</v>
@@ -1044,10 +1044,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C59">
         <v>2</v>
@@ -1055,10 +1055,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C60">
         <v>1</v>
@@ -1066,10 +1066,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -1077,10 +1077,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B62" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C62">
         <v>1</v>
@@ -1088,10 +1088,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C63">
         <v>2</v>
@@ -1099,10 +1099,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B64" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C64">
         <v>1</v>
@@ -1110,10 +1110,10 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C65">
         <v>2</v>
@@ -1121,10 +1121,10 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B66" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C66">
         <v>1</v>
@@ -1132,10 +1132,10 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C67">
         <v>2</v>
@@ -1143,10 +1143,10 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B68" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C68">
         <v>1</v>
@@ -1154,10 +1154,10 @@
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C69">
         <v>2</v>
@@ -1165,10 +1165,10 @@
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B70" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C70">
         <v>1</v>
@@ -1176,10 +1176,10 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C71">
         <v>2</v>
@@ -1187,10 +1187,10 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B72" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C72">
         <v>1</v>
@@ -1198,10 +1198,10 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C73">
         <v>2</v>
@@ -1209,10 +1209,10 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B74" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C74">
         <v>1</v>
@@ -1220,10 +1220,10 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C75">
         <v>2</v>
@@ -1231,10 +1231,10 @@
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B76" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -1242,10 +1242,10 @@
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C77">
         <v>2</v>
@@ -1253,10 +1253,10 @@
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B78" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C78">
         <v>1</v>
@@ -1264,10 +1264,10 @@
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C79">
         <v>2</v>
@@ -1275,10 +1275,10 @@
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B80" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C80">
         <v>1</v>
@@ -1286,10 +1286,10 @@
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C81">
         <v>2</v>
@@ -1297,10 +1297,10 @@
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B82" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C82">
         <v>1</v>
@@ -1308,10 +1308,10 @@
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C83">
         <v>2</v>
@@ -1319,10 +1319,10 @@
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B84" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C84">
         <v>1</v>
@@ -1330,10 +1330,10 @@
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C85">
         <v>2</v>
@@ -1341,10 +1341,10 @@
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B86" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C86">
         <v>1</v>
@@ -1352,10 +1352,10 @@
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C87">
         <v>2</v>
@@ -1363,10 +1363,10 @@
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B88" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C88">
         <v>1</v>
@@ -1374,10 +1374,10 @@
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C89">
         <v>2</v>
@@ -1385,10 +1385,10 @@
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B90" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C90">
         <v>1</v>
@@ -1396,10 +1396,10 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C91">
         <v>2</v>
@@ -1407,10 +1407,10 @@
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C92">
         <v>1</v>
@@ -1418,10 +1418,10 @@
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C93">
         <v>2</v>
@@ -1429,10 +1429,10 @@
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B94" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C94">
         <v>1</v>
@@ -1440,10 +1440,10 @@
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C95">
         <v>2</v>
@@ -1451,10 +1451,10 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B96" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C96">
         <v>1</v>
@@ -1462,10 +1462,10 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C97">
         <v>2</v>
@@ -1473,10 +1473,10 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B98" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C98">
         <v>1</v>
@@ -1484,10 +1484,10 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C99">
         <v>2</v>
@@ -1495,10 +1495,10 @@
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B100" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C100">
         <v>1</v>
@@ -1506,10 +1506,10 @@
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C101">
         <v>2</v>
@@ -1517,10 +1517,10 @@
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C102">
         <v>1</v>
@@ -1528,10 +1528,10 @@
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C103">
         <v>2</v>
@@ -1539,10 +1539,10 @@
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B104" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C104">
         <v>1</v>
@@ -1550,10 +1550,10 @@
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C105">
         <v>2</v>
@@ -1561,10 +1561,10 @@
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B106" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C106">
         <v>1</v>
@@ -1572,10 +1572,10 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C107">
         <v>2</v>
@@ -1583,10 +1583,10 @@
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C108">
         <v>1</v>
@@ -1594,10 +1594,10 @@
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C109">
         <v>2</v>
@@ -1605,10 +1605,10 @@
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B110" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C110">
         <v>1</v>
@@ -1616,10 +1616,10 @@
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C111">
         <v>2</v>
@@ -1627,10 +1627,10 @@
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B112" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C112">
         <v>1</v>
@@ -1638,10 +1638,10 @@
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C113">
         <v>2</v>
@@ -1649,10 +1649,10 @@
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B114" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C114">
         <v>1</v>
@@ -1660,10 +1660,10 @@
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C115">
         <v>2</v>
@@ -1671,10 +1671,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B116" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C116">
         <v>1</v>
@@ -1682,10 +1682,10 @@
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C117">
         <v>2</v>
@@ -1693,10 +1693,10 @@
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B118" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C118">
         <v>1</v>
@@ -1704,10 +1704,10 @@
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C119">
         <v>2</v>
@@ -1715,10 +1715,10 @@
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B120" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C120">
         <v>1</v>
@@ -1726,146 +1726,2214 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C121">
         <v>2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="1"/>
+      <c r="A122" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B122" t="s">
+        <v>6</v>
+      </c>
+      <c r="C122">
+        <v>1</v>
+      </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="1"/>
+      <c r="A123" t="s">
+        <v>6</v>
+      </c>
+      <c r="B123" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C123">
+        <v>2</v>
+      </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="1"/>
+      <c r="A124" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" t="s">
+        <v>6</v>
+      </c>
+      <c r="C124">
+        <v>1</v>
+      </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="1"/>
+      <c r="A125" t="s">
+        <v>6</v>
+      </c>
+      <c r="B125" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C125">
+        <v>2</v>
+      </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="1"/>
+      <c r="A126" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B126" t="s">
+        <v>6</v>
+      </c>
+      <c r="C126">
+        <v>1</v>
+      </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="1"/>
+      <c r="A127" t="s">
+        <v>6</v>
+      </c>
+      <c r="B127" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C127">
+        <v>2</v>
+      </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="1"/>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="1"/>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="1"/>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="1"/>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="1"/>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="1"/>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="1"/>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="1"/>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="1"/>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="1"/>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="1"/>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="1"/>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="1"/>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="1"/>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="1"/>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="1"/>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="1"/>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="1"/>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="1"/>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="1"/>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="1"/>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="1"/>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="1"/>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="1"/>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="1"/>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="1"/>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="1"/>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="1"/>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="1"/>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A157" s="1"/>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A158" s="1"/>
-    </row>
-    <row r="159" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A159" s="1"/>
-    </row>
-    <row r="160" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A160" s="1"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161" s="1"/>
-    </row>
-    <row r="162" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A162" s="1"/>
-    </row>
-    <row r="163" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A163" s="1"/>
-    </row>
-    <row r="164" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A164" s="1"/>
-    </row>
-    <row r="165" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A165" s="1"/>
+      <c r="A128" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B128" t="s">
+        <v>6</v>
+      </c>
+      <c r="C128">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" t="s">
+        <v>6</v>
+      </c>
+      <c r="B129" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C129">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B130" t="s">
+        <v>7</v>
+      </c>
+      <c r="C130">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" t="s">
+        <v>7</v>
+      </c>
+      <c r="B131" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C131">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132" t="s">
+        <v>7</v>
+      </c>
+      <c r="C132">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" t="s">
+        <v>7</v>
+      </c>
+      <c r="B133" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C133">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B134" t="s">
+        <v>7</v>
+      </c>
+      <c r="C134">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" t="s">
+        <v>7</v>
+      </c>
+      <c r="B135" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C135">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B136" t="s">
+        <v>7</v>
+      </c>
+      <c r="C136">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>7</v>
+      </c>
+      <c r="B137" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C137">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B138" t="s">
+        <v>7</v>
+      </c>
+      <c r="C138">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" t="s">
+        <v>7</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C139">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B140" t="s">
+        <v>7</v>
+      </c>
+      <c r="C140">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" t="s">
+        <v>7</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C141">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B142" t="s">
+        <v>7</v>
+      </c>
+      <c r="C142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>7</v>
+      </c>
+      <c r="B143" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C143">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B144" t="s">
+        <v>7</v>
+      </c>
+      <c r="C144">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" t="s">
+        <v>7</v>
+      </c>
+      <c r="B145" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C145">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B146" t="s">
+        <v>7</v>
+      </c>
+      <c r="C146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" t="s">
+        <v>7</v>
+      </c>
+      <c r="B147" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C147">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B148" t="s">
+        <v>7</v>
+      </c>
+      <c r="C148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>7</v>
+      </c>
+      <c r="B149" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C149">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B150" t="s">
+        <v>7</v>
+      </c>
+      <c r="C150">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" t="s">
+        <v>7</v>
+      </c>
+      <c r="B151" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C151">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B152" t="s">
+        <v>7</v>
+      </c>
+      <c r="C152">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" t="s">
+        <v>7</v>
+      </c>
+      <c r="B153" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C153">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B154" t="s">
+        <v>7</v>
+      </c>
+      <c r="C154">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" t="s">
+        <v>7</v>
+      </c>
+      <c r="B155" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B156" t="s">
+        <v>7</v>
+      </c>
+      <c r="C156">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" t="s">
+        <v>7</v>
+      </c>
+      <c r="B157" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B158" t="s">
+        <v>7</v>
+      </c>
+      <c r="C158">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
+        <v>7</v>
+      </c>
+      <c r="B159" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B160" t="s">
+        <v>7</v>
+      </c>
+      <c r="C160">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" t="s">
+        <v>7</v>
+      </c>
+      <c r="B161" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C161">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B162" t="s">
+        <v>7</v>
+      </c>
+      <c r="C162">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" t="s">
+        <v>7</v>
+      </c>
+      <c r="B163" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C163">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B164" t="s">
+        <v>7</v>
+      </c>
+      <c r="C164">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" t="s">
+        <v>7</v>
+      </c>
+      <c r="B165" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C165">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B166" t="s">
+        <v>7</v>
+      </c>
+      <c r="C166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" t="s">
+        <v>7</v>
+      </c>
+      <c r="B167" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C167">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B168" t="s">
+        <v>7</v>
+      </c>
+      <c r="C168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A169" t="s">
+        <v>7</v>
+      </c>
+      <c r="B169" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C169">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="170" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A170" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B170" t="s">
+        <v>7</v>
+      </c>
+      <c r="C170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A171" t="s">
+        <v>7</v>
+      </c>
+      <c r="B171" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C171">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B172" t="s">
+        <v>7</v>
+      </c>
+      <c r="C172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A173" t="s">
+        <v>7</v>
+      </c>
+      <c r="B173" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C173">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="174" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A174" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B174" t="s">
+        <v>7</v>
+      </c>
+      <c r="C174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A175" t="s">
+        <v>7</v>
+      </c>
+      <c r="B175" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C175">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="176" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A176" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B176" t="s">
+        <v>7</v>
+      </c>
+      <c r="C176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A177" t="s">
+        <v>7</v>
+      </c>
+      <c r="B177" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C177">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B178" t="s">
+        <v>7</v>
+      </c>
+      <c r="C178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A179" t="s">
+        <v>7</v>
+      </c>
+      <c r="B179" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C179">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A180" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B180" t="s">
+        <v>7</v>
+      </c>
+      <c r="C180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A181" t="s">
+        <v>7</v>
+      </c>
+      <c r="B181" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C181">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="182" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A182" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B182" t="s">
+        <v>7</v>
+      </c>
+      <c r="C182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A183" t="s">
+        <v>7</v>
+      </c>
+      <c r="B183" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C183">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="184" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A184" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B184" t="s">
+        <v>7</v>
+      </c>
+      <c r="C184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A185" t="s">
+        <v>7</v>
+      </c>
+      <c r="B185" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A186" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B186" t="s">
+        <v>7</v>
+      </c>
+      <c r="C186">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="187" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A187" t="s">
+        <v>7</v>
+      </c>
+      <c r="B187" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C187">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A188" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B188" t="s">
+        <v>7</v>
+      </c>
+      <c r="C188">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="189" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A189" t="s">
+        <v>7</v>
+      </c>
+      <c r="B189" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C189">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="190" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A190" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B190" t="s">
+        <v>7</v>
+      </c>
+      <c r="C190">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="191" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A191" t="s">
+        <v>7</v>
+      </c>
+      <c r="B191" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C191">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="192" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A192" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B192" t="s">
+        <v>7</v>
+      </c>
+      <c r="C192">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A193" t="s">
+        <v>7</v>
+      </c>
+      <c r="B193" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C193">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="194" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A194" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B194" t="s">
+        <v>8</v>
+      </c>
+      <c r="C194">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="195" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A195" t="s">
+        <v>8</v>
+      </c>
+      <c r="B195" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C195">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="196" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A196" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B196" t="s">
+        <v>8</v>
+      </c>
+      <c r="C196">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="197" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A197" t="s">
+        <v>8</v>
+      </c>
+      <c r="B197" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C197">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A198" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B198" t="s">
+        <v>8</v>
+      </c>
+      <c r="C198">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="199" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A199" t="s">
+        <v>8</v>
+      </c>
+      <c r="B199" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C199">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="200" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A200" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B200" t="s">
+        <v>8</v>
+      </c>
+      <c r="C200">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="201" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A201" t="s">
+        <v>8</v>
+      </c>
+      <c r="B201" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C201">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="202" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A202" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B202" t="s">
+        <v>8</v>
+      </c>
+      <c r="C202">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A203" t="s">
+        <v>8</v>
+      </c>
+      <c r="B203" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C203">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="204" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A204" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B204" t="s">
+        <v>8</v>
+      </c>
+      <c r="C204">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A205" t="s">
+        <v>8</v>
+      </c>
+      <c r="B205" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C205">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="206" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A206" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B206" t="s">
+        <v>8</v>
+      </c>
+      <c r="C206">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A207" t="s">
+        <v>8</v>
+      </c>
+      <c r="B207" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C207">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="208" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A208" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B208" t="s">
+        <v>8</v>
+      </c>
+      <c r="C208">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A209" t="s">
+        <v>8</v>
+      </c>
+      <c r="B209" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C209">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="210" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A210" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B210" t="s">
+        <v>8</v>
+      </c>
+      <c r="C210">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A211" t="s">
+        <v>8</v>
+      </c>
+      <c r="B211" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C211">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="212" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A212" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B212" t="s">
+        <v>8</v>
+      </c>
+      <c r="C212">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A213" t="s">
+        <v>8</v>
+      </c>
+      <c r="B213" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C213">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="214" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A214" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B214" t="s">
+        <v>8</v>
+      </c>
+      <c r="C214">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A215" t="s">
+        <v>8</v>
+      </c>
+      <c r="B215" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C215">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="216" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A216" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B216" t="s">
+        <v>8</v>
+      </c>
+      <c r="C216">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="217" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A217" t="s">
+        <v>8</v>
+      </c>
+      <c r="B217" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C217">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A218" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B218" t="s">
+        <v>8</v>
+      </c>
+      <c r="C218">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="219" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A219" t="s">
+        <v>8</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C219">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="220" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A220" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B220" t="s">
+        <v>8</v>
+      </c>
+      <c r="C220">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="221" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A221" t="s">
+        <v>8</v>
+      </c>
+      <c r="B221" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C221">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="222" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A222" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B222" t="s">
+        <v>8</v>
+      </c>
+      <c r="C222">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="223" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A223" t="s">
+        <v>8</v>
+      </c>
+      <c r="B223" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C223">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A224" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B224" t="s">
+        <v>8</v>
+      </c>
+      <c r="C224">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="225" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A225" t="s">
+        <v>8</v>
+      </c>
+      <c r="B225" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C225">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A226" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B226" t="s">
+        <v>8</v>
+      </c>
+      <c r="C226">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="227" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A227" t="s">
+        <v>8</v>
+      </c>
+      <c r="B227" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C227">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A228" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B228" t="s">
+        <v>8</v>
+      </c>
+      <c r="C228">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="229" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A229" t="s">
+        <v>8</v>
+      </c>
+      <c r="B229" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C229">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A230" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B230" t="s">
+        <v>8</v>
+      </c>
+      <c r="C230">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="231" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A231" t="s">
+        <v>8</v>
+      </c>
+      <c r="B231" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C231">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="232" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A232" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B232" t="s">
+        <v>8</v>
+      </c>
+      <c r="C232">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A233" t="s">
+        <v>8</v>
+      </c>
+      <c r="B233" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C233">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="234" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A234" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B234" t="s">
+        <v>8</v>
+      </c>
+      <c r="C234">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A235" t="s">
+        <v>8</v>
+      </c>
+      <c r="B235" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C235">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="236" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A236" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B236" t="s">
+        <v>8</v>
+      </c>
+      <c r="C236">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A237" t="s">
+        <v>8</v>
+      </c>
+      <c r="B237" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C237">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A238" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B238" t="s">
+        <v>8</v>
+      </c>
+      <c r="C238">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="239" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A239" t="s">
+        <v>8</v>
+      </c>
+      <c r="B239" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C239">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A240" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B240" t="s">
+        <v>8</v>
+      </c>
+      <c r="C240">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A241" t="s">
+        <v>8</v>
+      </c>
+      <c r="B241" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C241">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A242" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B242" t="s">
+        <v>8</v>
+      </c>
+      <c r="C242">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A243" t="s">
+        <v>8</v>
+      </c>
+      <c r="B243" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C243">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A244" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B244" t="s">
+        <v>8</v>
+      </c>
+      <c r="C244">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A245" t="s">
+        <v>8</v>
+      </c>
+      <c r="B245" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C245">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A246" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B246" t="s">
+        <v>8</v>
+      </c>
+      <c r="C246">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A247" t="s">
+        <v>8</v>
+      </c>
+      <c r="B247" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C247">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A248" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B248" t="s">
+        <v>8</v>
+      </c>
+      <c r="C248">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A249" t="s">
+        <v>8</v>
+      </c>
+      <c r="B249" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C249">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A250" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B250" t="s">
+        <v>8</v>
+      </c>
+      <c r="C250">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A251" t="s">
+        <v>8</v>
+      </c>
+      <c r="B251" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C251">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A252" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B252" t="s">
+        <v>8</v>
+      </c>
+      <c r="C252">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A253" t="s">
+        <v>8</v>
+      </c>
+      <c r="B253" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C253">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A254" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B254" t="s">
+        <v>8</v>
+      </c>
+      <c r="C254">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A255" t="s">
+        <v>8</v>
+      </c>
+      <c r="B255" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C255">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A256" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B256" t="s">
+        <v>8</v>
+      </c>
+      <c r="C256">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="257" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A257" t="s">
+        <v>8</v>
+      </c>
+      <c r="B257" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C257">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="258" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A258" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B258" t="s">
+        <v>4</v>
+      </c>
+      <c r="C258">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A259" t="s">
+        <v>4</v>
+      </c>
+      <c r="B259" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C259">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A260" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B260" t="s">
+        <v>4</v>
+      </c>
+      <c r="C260">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="261" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A261" t="s">
+        <v>4</v>
+      </c>
+      <c r="B261" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C261">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="262" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A262" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B262" t="s">
+        <v>4</v>
+      </c>
+      <c r="C262">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="263" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A263" t="s">
+        <v>4</v>
+      </c>
+      <c r="B263" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C263">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="264" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A264" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B264" t="s">
+        <v>4</v>
+      </c>
+      <c r="C264">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="265" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A265" t="s">
+        <v>4</v>
+      </c>
+      <c r="B265" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C265">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="266" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A266" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B266" t="s">
+        <v>4</v>
+      </c>
+      <c r="C266">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="267" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A267" t="s">
+        <v>4</v>
+      </c>
+      <c r="B267" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C267">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="268" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A268" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B268" t="s">
+        <v>4</v>
+      </c>
+      <c r="C268">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="269" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A269" t="s">
+        <v>4</v>
+      </c>
+      <c r="B269" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C269">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="270" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A270" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B270" t="s">
+        <v>4</v>
+      </c>
+      <c r="C270">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="271" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A271" t="s">
+        <v>4</v>
+      </c>
+      <c r="B271" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C271">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="272" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A272" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B272" t="s">
+        <v>4</v>
+      </c>
+      <c r="C272">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="273" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A273" t="s">
+        <v>4</v>
+      </c>
+      <c r="B273" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C273">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="274" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A274" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B274" t="s">
+        <v>4</v>
+      </c>
+      <c r="C274">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="275" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A275" t="s">
+        <v>4</v>
+      </c>
+      <c r="B275" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C275">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="276" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A276" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B276" t="s">
+        <v>4</v>
+      </c>
+      <c r="C276">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="277" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A277" t="s">
+        <v>4</v>
+      </c>
+      <c r="B277" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C277">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="278" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A278" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B278" t="s">
+        <v>4</v>
+      </c>
+      <c r="C278">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="279" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A279" t="s">
+        <v>4</v>
+      </c>
+      <c r="B279" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C279">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="280" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A280" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B280" t="s">
+        <v>4</v>
+      </c>
+      <c r="C280">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="281" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A281" t="s">
+        <v>4</v>
+      </c>
+      <c r="B281" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C281">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="282" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A282" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B282" t="s">
+        <v>4</v>
+      </c>
+      <c r="C282">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="283" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A283" t="s">
+        <v>4</v>
+      </c>
+      <c r="B283" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C283">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="284" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A284" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B284" t="s">
+        <v>4</v>
+      </c>
+      <c r="C284">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="285" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A285" t="s">
+        <v>4</v>
+      </c>
+      <c r="B285" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C285">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="286" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A286" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B286" t="s">
+        <v>4</v>
+      </c>
+      <c r="C286">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="287" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A287" t="s">
+        <v>4</v>
+      </c>
+      <c r="B287" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C287">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="288" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A288" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B288" t="s">
+        <v>4</v>
+      </c>
+      <c r="C288">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A289" t="s">
+        <v>4</v>
+      </c>
+      <c r="B289" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C289">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A290" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B290" t="s">
+        <v>4</v>
+      </c>
+      <c r="C290">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="291" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>4</v>
+      </c>
+      <c r="B291" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C291">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B292" t="s">
+        <v>4</v>
+      </c>
+      <c r="C292">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>4</v>
+      </c>
+      <c r="B293" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C293">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B294" t="s">
+        <v>4</v>
+      </c>
+      <c r="C294">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>4</v>
+      </c>
+      <c r="B295" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C295">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="296" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A296" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B296" t="s">
+        <v>4</v>
+      </c>
+      <c r="C296">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="297" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>4</v>
+      </c>
+      <c r="B297" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C297">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="298" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A298" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B298" t="s">
+        <v>4</v>
+      </c>
+      <c r="C298">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="299" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A299" t="s">
+        <v>4</v>
+      </c>
+      <c r="B299" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C299">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="300" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A300" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B300" t="s">
+        <v>4</v>
+      </c>
+      <c r="C300">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="301" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A301" t="s">
+        <v>4</v>
+      </c>
+      <c r="B301" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C301">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="302" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A302" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B302" t="s">
+        <v>4</v>
+      </c>
+      <c r="C302">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="303" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>4</v>
+      </c>
+      <c r="B303" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C303">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="304" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A304" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B304" t="s">
+        <v>4</v>
+      </c>
+      <c r="C304">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="305" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A305" t="s">
+        <v>4</v>
+      </c>
+      <c r="B305" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C305">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="306" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A306" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B306" t="s">
+        <v>4</v>
+      </c>
+      <c r="C306">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="307" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A307" t="s">
+        <v>4</v>
+      </c>
+      <c r="B307" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C307">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="308" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A308" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B308" t="s">
+        <v>4</v>
+      </c>
+      <c r="C308">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="309" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A309" t="s">
+        <v>4</v>
+      </c>
+      <c r="B309" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C309">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="310" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A310" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B310" t="s">
+        <v>4</v>
+      </c>
+      <c r="C310">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="311" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A311" t="s">
+        <v>4</v>
+      </c>
+      <c r="B311" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C311">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="312" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A312" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B312" t="s">
+        <v>4</v>
+      </c>
+      <c r="C312">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="313" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A313" t="s">
+        <v>4</v>
+      </c>
+      <c r="B313" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C313">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="314" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A314" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B314" t="s">
+        <v>4</v>
+      </c>
+      <c r="C314">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="315" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A315" t="s">
+        <v>4</v>
+      </c>
+      <c r="B315" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C315">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="316" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A316" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B316" t="s">
+        <v>4</v>
+      </c>
+      <c r="C316">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="317" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A317" t="s">
+        <v>4</v>
+      </c>
+      <c r="B317" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C317">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="318" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A318" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B318" t="s">
+        <v>4</v>
+      </c>
+      <c r="C318">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="319" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A319" t="s">
+        <v>4</v>
+      </c>
+      <c r="B319" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C319">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="320" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A320" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B320" t="s">
+        <v>4</v>
+      </c>
+      <c r="C320">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="321" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>4</v>
+      </c>
+      <c r="B321" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C321">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>